<commit_message>
Week 10 and Women Tell All Update
</commit_message>
<xml_diff>
--- a/Bachelor Fantasy 2017.xlsx
+++ b/Bachelor Fantasy 2017.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
   <si>
     <t>Team</t>
   </si>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>Eliminated</t>
-  </si>
-  <si>
-    <t>Still in it to Win it</t>
   </si>
 </sst>
 </file>
@@ -595,7 +592,7 @@
       </c>
       <c r="L2">
         <f>VLOOKUP(B2,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M2">
         <f>VLOOKUP(B2,Contestants!$A$2:$M$13,12,FALSE)</f>
@@ -607,7 +604,7 @@
       </c>
       <c r="O2">
         <f>SUM(C2:M2)</f>
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -655,7 +652,7 @@
       </c>
       <c r="L3">
         <f>VLOOKUP(B3,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M3">
         <f>VLOOKUP(B3,Contestants!$A$2:$M$13,12,FALSE)</f>
@@ -667,7 +664,7 @@
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O21" si="0">SUM(C3:M3)</f>
-        <v>420</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -775,7 +772,7 @@
       </c>
       <c r="L5">
         <f>VLOOKUP(B5,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M5">
         <f>VLOOKUP(B5,Contestants!$A$2:$M$13,12,FALSE)</f>
@@ -787,7 +784,7 @@
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>415</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -895,7 +892,7 @@
       </c>
       <c r="L7">
         <f>VLOOKUP(B7,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M7">
         <f>VLOOKUP(B7,Contestants!$A$2:$M$13,12,FALSE)</f>
@@ -907,7 +904,7 @@
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -955,19 +952,19 @@
       </c>
       <c r="L8">
         <f>VLOOKUP(B8,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M8">
         <f>VLOOKUP(B8,Contestants!$A$2:$M$13,12,FALSE)</f>
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="N8" t="str">
         <f>VLOOKUP(B8,Contestants!$A$2:$M$13,13,FALSE)</f>
-        <v>Still in it to Win it</v>
+        <v>Eliminated</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>540</v>
+        <v>700</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1015,7 +1012,7 @@
       </c>
       <c r="L9">
         <f>VLOOKUP(B9,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M9">
         <f>VLOOKUP(B9,Contestants!$A$2:$M$13,12,FALSE)</f>
@@ -1027,7 +1024,7 @@
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>750</v>
+        <v>795</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1075,7 +1072,7 @@
       </c>
       <c r="L10">
         <f>VLOOKUP(B10,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M10">
         <f>VLOOKUP(B10,Contestants!$A$2:$M$13,12,FALSE)</f>
@@ -1087,7 +1084,7 @@
       </c>
       <c r="O10">
         <f t="shared" si="0"/>
-        <v>420</v>
+        <v>425</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1135,7 +1132,7 @@
       </c>
       <c r="L11">
         <f>VLOOKUP(B11,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M11">
         <f>VLOOKUP(B11,Contestants!$A$2:$M$13,12,FALSE)</f>
@@ -1147,7 +1144,7 @@
       </c>
       <c r="O11">
         <f t="shared" si="0"/>
-        <v>430</v>
+        <v>475</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1255,7 +1252,7 @@
       </c>
       <c r="L13">
         <f>VLOOKUP(B13,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M13">
         <f>VLOOKUP(B13,Contestants!$A$2:$M$13,12,FALSE)</f>
@@ -1267,7 +1264,7 @@
       </c>
       <c r="O13">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1435,7 +1432,7 @@
       </c>
       <c r="L16">
         <f>VLOOKUP(B16,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M16">
         <f>VLOOKUP(B16,Contestants!$A$2:$M$13,12,FALSE)</f>
@@ -1447,7 +1444,7 @@
       </c>
       <c r="O16">
         <f t="shared" si="0"/>
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1555,7 +1552,7 @@
       </c>
       <c r="L18">
         <f>VLOOKUP(B18,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M18">
         <f>VLOOKUP(B18,Contestants!$A$2:$M$13,12,FALSE)</f>
@@ -1567,7 +1564,7 @@
       </c>
       <c r="O18">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1615,7 +1612,7 @@
       </c>
       <c r="L19">
         <f>VLOOKUP(B19,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M19">
         <f>VLOOKUP(B19,Contestants!$A$2:$M$13,12,FALSE)</f>
@@ -1627,7 +1624,7 @@
       </c>
       <c r="O19">
         <f t="shared" si="0"/>
-        <v>420</v>
+        <v>425</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1735,7 +1732,7 @@
       </c>
       <c r="L21">
         <f>VLOOKUP(B21,Contestants!$A$2:$M$13,11,FALSE)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M21">
         <f>VLOOKUP(B21,Contestants!$A$2:$M$13,12,FALSE)</f>
@@ -1747,7 +1744,7 @@
       </c>
       <c r="O21">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1761,12 +1758,13 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1883,7 +1881,7 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1924,7 +1922,7 @@
         <v>45</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1965,7 +1963,7 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -2006,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -2088,7 +2086,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -2170,7 +2168,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -2252,13 +2250,13 @@
         <v>45</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="M12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2293,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L13">
         <v>0</v>

</xml_diff>